<commit_message>
Fixed GPIO, system, added soctest file
</commit_message>
<xml_diff>
--- a/Recursive vs. Factorial Data.xlsx
+++ b/Recursive vs. Factorial Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Documents\SJSU\Fall 2019\CMPE 140\CMPE-140-Assignment-8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9093F64-8613-4FCF-9019-16F54D158B2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D19430-C11F-4F4F-9ED9-B68C15A0DD42}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0BFA6502-D9CA-4377-942F-7F4AF75EE5F8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>n</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>*4 clocks to Error</t>
+  </si>
+  <si>
+    <t>#update ACCEL to take also include the cycles to load within n and catch n! within the CPU</t>
   </si>
 </sst>
 </file>
@@ -66,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -117,11 +120,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -129,6 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1422,16 +1435,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
+      <xdr:colOff>411480</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1777,6 +1790,9 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="2">

</xml_diff>

<commit_message>
updated instruction memory file to run factorial accelerator method
</commit_message>
<xml_diff>
--- a/Recursive vs. Factorial Data.xlsx
+++ b/Recursive vs. Factorial Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work\Documents\SJSU\Fall 2019\CMPE 140\CMPE-140-Assignment-8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D19430-C11F-4F4F-9ED9-B68C15A0DD42}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6097A9-7587-4488-BD61-48709C892246}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0BFA6502-D9CA-4377-942F-7F4AF75EE5F8}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>n</t>
   </si>
@@ -46,6 +46,39 @@
   </si>
   <si>
     <t>#update ACCEL to take also include the cycles to load within n and catch n! within the CPU</t>
+  </si>
+  <si>
+    <t>load n</t>
+  </si>
+  <si>
+    <t>load go</t>
+  </si>
+  <si>
+    <t>send n</t>
+  </si>
+  <si>
+    <t>send go</t>
+  </si>
+  <si>
+    <t>read done</t>
+  </si>
+  <si>
+    <t>read nf</t>
+  </si>
+  <si>
+    <t>store nf</t>
+  </si>
+  <si>
+    <t>branch if done or error</t>
+  </si>
+  <si>
+    <t>branch to factorial</t>
+  </si>
+  <si>
+    <t>wait till return</t>
+  </si>
+  <si>
+    <t>store return value</t>
   </si>
 </sst>
 </file>
@@ -480,52 +513,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>28</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>32</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1769,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26CAA35-B19A-4A17-A58D-224B97AFB34F}">
-  <dimension ref="B2:E18"/>
+  <dimension ref="B2:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1802,7 +1835,8 @@
         <v>12</v>
       </c>
       <c r="D3" s="2">
-        <v>6</v>
+        <f>8+6</f>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -1813,7 +1847,8 @@
         <v>12</v>
       </c>
       <c r="D4" s="1">
-        <v>8</v>
+        <f>8+8</f>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -1824,7 +1859,8 @@
         <v>26</v>
       </c>
       <c r="D5" s="1">
-        <v>12</v>
+        <f>8+12</f>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -1835,7 +1871,8 @@
         <v>40</v>
       </c>
       <c r="D6" s="1">
-        <v>14</v>
+        <f>8+14</f>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -1846,7 +1883,8 @@
         <v>54</v>
       </c>
       <c r="D7" s="1">
-        <v>16</v>
+        <f>8+16</f>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
@@ -1857,7 +1895,8 @@
         <v>68</v>
       </c>
       <c r="D8" s="1">
-        <v>18</v>
+        <f>8+18</f>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
@@ -1868,7 +1907,8 @@
         <v>82</v>
       </c>
       <c r="D9" s="1">
-        <v>20</v>
+        <f>8+20</f>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
@@ -1879,7 +1919,8 @@
         <v>96</v>
       </c>
       <c r="D10" s="1">
-        <v>22</v>
+        <f>8+22</f>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
@@ -1890,7 +1931,8 @@
         <v>110</v>
       </c>
       <c r="D11" s="1">
-        <v>24</v>
+        <f>8+24</f>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
@@ -1912,7 +1954,8 @@
         <v>138</v>
       </c>
       <c r="D13" s="1">
-        <v>28</v>
+        <f>8+28</f>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
@@ -1923,7 +1966,8 @@
         <v>152</v>
       </c>
       <c r="D14" s="1">
-        <v>30</v>
+        <f>8+30</f>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
@@ -1934,7 +1978,8 @@
         <v>166</v>
       </c>
       <c r="D15" s="1">
-        <v>32</v>
+        <f>8+32</f>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
@@ -1945,7 +1990,8 @@
         <v>182</v>
       </c>
       <c r="D16" s="1">
-        <v>4</v>
+        <f>8+4</f>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
@@ -1959,7 +2005,8 @@
         <v>194</v>
       </c>
       <c r="D17" s="1">
-        <v>4</v>
+        <f>8+4</f>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
         <v>3</v>
@@ -1973,10 +2020,63 @@
         <v>208</v>
       </c>
       <c r="D18" s="1">
-        <v>4</v>
+        <f>8+4</f>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>